<commit_message>
endpoint GET con filtros básicos, sort, skip y limit
</commit_message>
<xml_diff>
--- a/CRONOPLAST_100622(1).xlsx
+++ b/CRONOPLAST_100622(1).xlsx
@@ -456,10 +456,10 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.87"/>

</xml_diff>